<commit_message>
Finished Q3 and Q4
</commit_message>
<xml_diff>
--- a/2018-QS-World-University-Rankings-Top200-edited.xlsx
+++ b/2018-QS-World-University-Rankings-Top200-edited.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB5C985-22F9-4A4C-A1BA-6E70023DF025}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611C8DBE-A04E-466A-B7A1-6B637FA8BEF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4155" yWindow="4155" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1099,27 +1121,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J207"/>
+  <dimension ref="A1:J210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
-      <selection activeCell="C208" sqref="C208"/>
+    <sheetView tabSelected="1" topLeftCell="B200" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="E205" sqref="E205"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.921875" customWidth="1"/>
-    <col min="2" max="2" width="13.61328125" customWidth="1"/>
-    <col min="3" max="3" width="8.15234375" customWidth="1"/>
-    <col min="4" max="4" width="18.07421875" customWidth="1"/>
-    <col min="5" max="5" width="18.23046875" customWidth="1"/>
-    <col min="6" max="6" width="14.07421875" customWidth="1"/>
-    <col min="7" max="7" width="17.53515625" customWidth="1"/>
-    <col min="8" max="8" width="17.69140625" customWidth="1"/>
-    <col min="9" max="9" width="19.15234375" customWidth="1"/>
-    <col min="10" max="10" width="12.69140625" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>234</v>
       </c>
@@ -1151,7 +1173,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1183,7 +1205,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1215,7 +1237,7 @@
         <v>98.7</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1247,7 +1269,7 @@
         <v>98.4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1279,7 +1301,7 @@
         <v>97.7</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1311,7 +1333,7 @@
         <v>95.6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1343,7 +1365,7 @@
         <v>95.3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1375,7 +1397,7 @@
         <v>94.6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1407,7 +1429,7 @@
         <v>93.7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1439,7 +1461,7 @@
         <v>93.5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1471,7 +1493,7 @@
         <v>93.3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1503,7 +1525,7 @@
         <v>92.2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1535,7 +1557,7 @@
         <v>91.2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1567,7 +1589,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1599,7 +1621,7 @@
         <v>90.7</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1631,7 +1653,7 @@
         <v>90.5</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1663,7 +1685,7 @@
         <v>90.4</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1695,7 +1717,7 @@
         <v>89.8</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1727,7 +1749,7 @@
         <v>88.9</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1759,7 +1781,7 @@
         <v>88.7</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1791,7 +1813,7 @@
         <v>87.1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1823,7 +1845,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1855,7 +1877,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1887,7 +1909,7 @@
         <v>86.9</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1919,7 +1941,7 @@
         <v>86.9</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1951,7 +1973,7 @@
         <v>85.6</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1983,7 +2005,7 @@
         <v>85.5</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2015,7 +2037,7 @@
         <v>84.9</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -2047,7 +2069,7 @@
         <v>84.8</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -2079,7 +2101,7 @@
         <v>84.8</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2111,7 +2133,7 @@
         <v>84.3</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2143,7 +2165,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -2175,7 +2197,7 @@
         <v>83.9</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -2207,7 +2229,7 @@
         <v>83.6</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -2239,7 +2261,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -2271,7 +2293,7 @@
         <v>81.8</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -2303,7 +2325,7 @@
         <v>81.5</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -2335,7 +2357,7 @@
         <v>81.5</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -2367,7 +2389,7 @@
         <v>80.8</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -2399,7 +2421,7 @@
         <v>80.8</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -2431,7 +2453,7 @@
         <v>80.599999999999994</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -2463,7 +2485,7 @@
         <v>80.400000000000006</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -2495,7 +2517,7 @@
         <v>80.400000000000006</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2527,7 +2549,7 @@
         <v>79.900000000000006</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -2559,7 +2581,7 @@
         <v>79.5</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -2591,7 +2613,7 @@
         <v>78.900000000000006</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -2623,7 +2645,7 @@
         <v>78.8</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -2655,7 +2677,7 @@
         <v>78.599999999999994</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -2687,7 +2709,7 @@
         <v>78.599999999999994</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2719,7 +2741,7 @@
         <v>78.400000000000006</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -2751,7 +2773,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -2783,7 +2805,7 @@
         <v>77.900000000000006</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -2815,7 +2837,7 @@
         <v>77.3</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -2847,7 +2869,7 @@
         <v>76.5</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -2879,7 +2901,7 @@
         <v>76.099999999999994</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -2911,7 +2933,7 @@
         <v>75.8</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -2943,7 +2965,7 @@
         <v>74.8</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -2975,7 +2997,7 @@
         <v>74.400000000000006</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -3007,7 +3029,7 @@
         <v>74.3</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -3039,7 +3061,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -3071,7 +3093,7 @@
         <v>73.099999999999994</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -3103,7 +3125,7 @@
         <v>72.900000000000006</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -3135,7 +3157,7 @@
         <v>72.5</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -3167,7 +3189,7 @@
         <v>72.099999999999994</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>63</v>
       </c>
@@ -3199,7 +3221,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>64</v>
       </c>
@@ -3231,7 +3253,7 @@
         <v>71.599999999999994</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>65</v>
       </c>
@@ -3263,7 +3285,7 @@
         <v>70.8</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -3295,7 +3317,7 @@
         <v>70.599999999999994</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>67</v>
       </c>
@@ -3327,7 +3349,7 @@
         <v>70.400000000000006</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -3359,7 +3381,7 @@
         <v>70.3</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -3391,7 +3413,7 @@
         <v>70.099999999999994</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -3423,7 +3445,7 @@
         <v>69.400000000000006</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>71</v>
       </c>
@@ -3455,7 +3477,7 @@
         <v>69.400000000000006</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -3487,7 +3509,7 @@
         <v>69.2</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>73</v>
       </c>
@@ -3519,7 +3541,7 @@
         <v>69.2</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -3551,7 +3573,7 @@
         <v>69.099999999999994</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -3583,7 +3605,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -3615,7 +3637,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>77</v>
       </c>
@@ -3647,7 +3669,7 @@
         <v>68.5</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -3679,7 +3701,7 @@
         <v>68.5</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>79</v>
       </c>
@@ -3711,7 +3733,7 @@
         <v>67.8</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>80</v>
       </c>
@@ -3743,7 +3765,7 @@
         <v>67.2</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>81</v>
       </c>
@@ -3775,7 +3797,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -3807,7 +3829,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>83</v>
       </c>
@@ -3839,7 +3861,7 @@
         <v>66.8</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>84</v>
       </c>
@@ -3871,7 +3893,7 @@
         <v>66.8</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>85</v>
       </c>
@@ -3903,7 +3925,7 @@
         <v>66.099999999999994</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>86</v>
       </c>
@@ -3935,7 +3957,7 @@
         <v>65.900000000000006</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>87</v>
       </c>
@@ -3967,7 +3989,7 @@
         <v>65.7</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>88</v>
       </c>
@@ -3999,7 +4021,7 @@
         <v>65.599999999999994</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>89</v>
       </c>
@@ -4031,7 +4053,7 @@
         <v>65.5</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>90</v>
       </c>
@@ -4063,7 +4085,7 @@
         <v>65.5</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -4095,7 +4117,7 @@
         <v>65.3</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>92</v>
       </c>
@@ -4127,7 +4149,7 @@
         <v>65.2</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>93</v>
       </c>
@@ -4159,7 +4181,7 @@
         <v>65.2</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>94</v>
       </c>
@@ -4191,7 +4213,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -4223,7 +4245,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>96</v>
       </c>
@@ -4255,7 +4277,7 @@
         <v>64.900000000000006</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -4287,7 +4309,7 @@
         <v>64.7</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>98</v>
       </c>
@@ -4319,7 +4341,7 @@
         <v>64.7</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>99</v>
       </c>
@@ -4351,7 +4373,7 @@
         <v>64.599999999999994</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>100</v>
       </c>
@@ -4383,7 +4405,7 @@
         <v>64.5</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>101</v>
       </c>
@@ -4415,7 +4437,7 @@
         <v>63.9</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>102</v>
       </c>
@@ -4447,7 +4469,7 @@
         <v>63.9</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>103</v>
       </c>
@@ -4479,7 +4501,7 @@
         <v>63.6</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>104</v>
       </c>
@@ -4511,7 +4533,7 @@
         <v>63.2</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>105</v>
       </c>
@@ -4543,7 +4565,7 @@
         <v>62.3</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>106</v>
       </c>
@@ -4575,7 +4597,7 @@
         <v>61.9</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>107</v>
       </c>
@@ -4607,7 +4629,7 @@
         <v>61.6</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>108</v>
       </c>
@@ -4639,7 +4661,7 @@
         <v>61.5</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>109</v>
       </c>
@@ -4671,7 +4693,7 @@
         <v>61.5</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>110</v>
       </c>
@@ -4703,7 +4725,7 @@
         <v>61.5</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>111</v>
       </c>
@@ -4735,7 +4757,7 @@
         <v>61.4</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>112</v>
       </c>
@@ -4767,7 +4789,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>113</v>
       </c>
@@ -4799,7 +4821,7 @@
         <v>60.8</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>114</v>
       </c>
@@ -4831,7 +4853,7 @@
         <v>60.8</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>115</v>
       </c>
@@ -4863,7 +4885,7 @@
         <v>60.7</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>116</v>
       </c>
@@ -4895,7 +4917,7 @@
         <v>60.7</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>117</v>
       </c>
@@ -4927,7 +4949,7 @@
         <v>60.4</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>118</v>
       </c>
@@ -4959,7 +4981,7 @@
         <v>59.3</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>119</v>
       </c>
@@ -4991,7 +5013,7 @@
         <v>59.2</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>120</v>
       </c>
@@ -5023,7 +5045,7 @@
         <v>59.1</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>121</v>
       </c>
@@ -5055,7 +5077,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>122</v>
       </c>
@@ -5087,7 +5109,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>123</v>
       </c>
@@ -5119,7 +5141,7 @@
         <v>58.7</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>124</v>
       </c>
@@ -5151,7 +5173,7 @@
         <v>58.4</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>125</v>
       </c>
@@ -5183,7 +5205,7 @@
         <v>58.4</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>126</v>
       </c>
@@ -5215,7 +5237,7 @@
         <v>58.3</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>127</v>
       </c>
@@ -5247,7 +5269,7 @@
         <v>58.2</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>128</v>
       </c>
@@ -5279,7 +5301,7 @@
         <v>58.1</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>129</v>
       </c>
@@ -5311,7 +5333,7 @@
         <v>57.7</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>130</v>
       </c>
@@ -5343,7 +5365,7 @@
         <v>57.5</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>131</v>
       </c>
@@ -5375,7 +5397,7 @@
         <v>57.2</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>132</v>
       </c>
@@ -5407,7 +5429,7 @@
         <v>57.1</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>133</v>
       </c>
@@ -5439,7 +5461,7 @@
         <v>56.9</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>134</v>
       </c>
@@ -5471,7 +5493,7 @@
         <v>56.3</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>135</v>
       </c>
@@ -5503,7 +5525,7 @@
         <v>56.3</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>136</v>
       </c>
@@ -5535,7 +5557,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>137</v>
       </c>
@@ -5567,7 +5589,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>138</v>
       </c>
@@ -5599,7 +5621,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>139</v>
       </c>
@@ -5631,7 +5653,7 @@
         <v>55.8</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>140</v>
       </c>
@@ -5663,7 +5685,7 @@
         <v>55.6</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>141</v>
       </c>
@@ -5695,7 +5717,7 @@
         <v>55.5</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>142</v>
       </c>
@@ -5727,7 +5749,7 @@
         <v>55.5</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>143</v>
       </c>
@@ -5759,7 +5781,7 @@
         <v>55.2</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>144</v>
       </c>
@@ -5791,7 +5813,7 @@
         <v>54.7</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>145</v>
       </c>
@@ -5823,7 +5845,7 @@
         <v>54.5</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>146</v>
       </c>
@@ -5855,7 +5877,7 @@
         <v>54.4</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>147</v>
       </c>
@@ -5887,7 +5909,7 @@
         <v>54.4</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>148</v>
       </c>
@@ -5919,7 +5941,7 @@
         <v>54.3</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>149</v>
       </c>
@@ -5951,7 +5973,7 @@
         <v>54.3</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>150</v>
       </c>
@@ -5983,7 +6005,7 @@
         <v>54.2</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>151</v>
       </c>
@@ -6015,7 +6037,7 @@
         <v>53.7</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>152</v>
       </c>
@@ -6047,7 +6069,7 @@
         <v>53.6</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>153</v>
       </c>
@@ -6079,7 +6101,7 @@
         <v>53.3</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>154</v>
       </c>
@@ -6111,7 +6133,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>155</v>
       </c>
@@ -6143,7 +6165,7 @@
         <v>52.9</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>156</v>
       </c>
@@ -6175,7 +6197,7 @@
         <v>52.8</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>157</v>
       </c>
@@ -6207,7 +6229,7 @@
         <v>52.7</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>158</v>
       </c>
@@ -6239,7 +6261,7 @@
         <v>52.7</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>159</v>
       </c>
@@ -6271,7 +6293,7 @@
         <v>52.6</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>160</v>
       </c>
@@ -6303,7 +6325,7 @@
         <v>52.4</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>161</v>
       </c>
@@ -6335,7 +6357,7 @@
         <v>52.4</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>162</v>
       </c>
@@ -6367,7 +6389,7 @@
         <v>52.2</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>163</v>
       </c>
@@ -6399,7 +6421,7 @@
         <v>52.1</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>164</v>
       </c>
@@ -6431,7 +6453,7 @@
         <v>52.1</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>165</v>
       </c>
@@ -6463,7 +6485,7 @@
         <v>52.1</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>166</v>
       </c>
@@ -6495,7 +6517,7 @@
         <v>51.9</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>167</v>
       </c>
@@ -6527,7 +6549,7 @@
         <v>51.5</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>168</v>
       </c>
@@ -6559,7 +6581,7 @@
         <v>51.3</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>169</v>
       </c>
@@ -6591,7 +6613,7 @@
         <v>50.9</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>170</v>
       </c>
@@ -6623,7 +6645,7 @@
         <v>50.8</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>171</v>
       </c>
@@ -6655,7 +6677,7 @@
         <v>50.7</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>172</v>
       </c>
@@ -6687,7 +6709,7 @@
         <v>50.3</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>173</v>
       </c>
@@ -6719,7 +6741,7 @@
         <v>50.3</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>174</v>
       </c>
@@ -6751,7 +6773,7 @@
         <v>50.3</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>175</v>
       </c>
@@ -6783,7 +6805,7 @@
         <v>50.1</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>176</v>
       </c>
@@ -6815,7 +6837,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>177</v>
       </c>
@@ -6847,7 +6869,7 @@
         <v>49.8</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>178</v>
       </c>
@@ -6879,7 +6901,7 @@
         <v>49.7</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>179</v>
       </c>
@@ -6911,7 +6933,7 @@
         <v>49.7</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>180</v>
       </c>
@@ -6943,7 +6965,7 @@
         <v>49.6</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>181</v>
       </c>
@@ -6975,7 +6997,7 @@
         <v>49.5</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>182</v>
       </c>
@@ -7007,7 +7029,7 @@
         <v>49.5</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>183</v>
       </c>
@@ -7039,7 +7061,7 @@
         <v>49.5</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>184</v>
       </c>
@@ -7071,7 +7093,7 @@
         <v>49.5</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>185</v>
       </c>
@@ -7103,7 +7125,7 @@
         <v>49.3</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>186</v>
       </c>
@@ -7135,7 +7157,7 @@
         <v>49.2</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>187</v>
       </c>
@@ -7167,7 +7189,7 @@
         <v>49.1</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>188</v>
       </c>
@@ -7199,7 +7221,7 @@
         <v>49.1</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>189</v>
       </c>
@@ -7231,7 +7253,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>190</v>
       </c>
@@ -7263,7 +7285,7 @@
         <v>48.9</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>191</v>
       </c>
@@ -7295,7 +7317,7 @@
         <v>48.5</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>192</v>
       </c>
@@ -7327,7 +7349,7 @@
         <v>48.5</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>193</v>
       </c>
@@ -7359,7 +7381,7 @@
         <v>48.5</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>194</v>
       </c>
@@ -7391,7 +7413,7 @@
         <v>48.1</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>195</v>
       </c>
@@ -7423,7 +7445,7 @@
         <v>48.1</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>196</v>
       </c>
@@ -7455,7 +7477,7 @@
         <v>48.1</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>197</v>
       </c>
@@ -7487,7 +7509,7 @@
         <v>48.1</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>198</v>
       </c>
@@ -7519,7 +7541,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>199</v>
       </c>
@@ -7551,7 +7573,7 @@
         <v>47.9</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C202" t="s">
         <v>248</v>
       </c>
@@ -7560,7 +7582,7 @@
         <v>18.8</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C203" t="s">
         <v>247</v>
       </c>
@@ -7569,16 +7591,20 @@
         <v>72.324500000000029</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C204" t="s">
         <v>246</v>
       </c>
       <c r="D204">
-        <f>_xlfn.STDEV.P(D2:D201)</f>
-        <v>21.24817520988552</v>
-      </c>
-    </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.4">
+        <f>_xlfn.STDEV.S(D2:D201)</f>
+        <v>21.301495683207364</v>
+      </c>
+      <c r="E204" t="e" cm="1">
+        <f t="array" ref="E204">STDEV</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C205" t="s">
         <v>245</v>
       </c>
@@ -7587,7 +7613,7 @@
         <v>21.301495683207364</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C206" t="s">
         <v>249</v>
       </c>
@@ -7596,12 +7622,30 @@
         <v>200</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C207" t="s">
         <v>250</v>
       </c>
       <c r="D207">
         <v>1.96</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D208">
+        <f>CONFIDENCE(0.05,D204,D206)</f>
+        <v>2.9521824331725233</v>
+      </c>
+    </row>
+    <row r="209" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D209">
+        <f>ROUND(D203-D208,2)</f>
+        <v>69.37</v>
+      </c>
+    </row>
+    <row r="210" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D210">
+        <f>ROUND(D203+D208,2)</f>
+        <v>75.28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>